<commit_message>
Expands on excel spreadsheet config files. Runs each config and outputs results to excel sheet named for that run.  Future plans to have all data for a single run on one sheet and add sheets to single excel file
</commit_message>
<xml_diff>
--- a/SchedSimConfig.xlsx
+++ b/SchedSimConfig.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Patients</t>
   </si>
@@ -416,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,6 +487,35 @@
         <v>0.1</v>
       </c>
     </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>90</v>
+      </c>
+      <c r="B3">
+        <v>50</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>0.4</v>
+      </c>
+      <c r="F3">
+        <v>0.25</v>
+      </c>
+      <c r="G3">
+        <v>0.15</v>
+      </c>
+      <c r="H3">
+        <v>0.1</v>
+      </c>
+      <c r="I3">
+        <v>0.1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Refines counting of appointments attended, adds states to patients
</commit_message>
<xml_diff>
--- a/SchedSimConfig.xlsx
+++ b/SchedSimConfig.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Patients</t>
   </si>
@@ -416,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A3" sqref="A3:I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,35 +487,6 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>90</v>
-      </c>
-      <c r="B3">
-        <v>50</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>0.4</v>
-      </c>
-      <c r="F3">
-        <v>0.25</v>
-      </c>
-      <c r="G3">
-        <v>0.15</v>
-      </c>
-      <c r="H3">
-        <v>0.1</v>
-      </c>
-      <c r="I3">
-        <v>0.1</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Simplifies log outputs, adds configurable days in week to simulate, refines cancellations and revelation of cancellations
</commit_message>
<xml_diff>
--- a/SchedSimConfig.xlsx
+++ b/SchedSimConfig.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Patients</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>PctRel28</t>
+  </si>
+  <si>
+    <t>DaysInCycle</t>
   </si>
 </sst>
 </file>
@@ -416,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:I4"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,9 +430,10 @@
     <col min="1" max="1" width="19" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="10" max="10" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -457,10 +461,13 @@
       <c r="I1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>180</v>
+        <v>100</v>
       </c>
       <c r="B2">
         <v>100</v>
@@ -485,6 +492,9 @@
       </c>
       <c r="I2">
         <v>0.1</v>
+      </c>
+      <c r="J2">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rearranges metrics data, adds follow-up probability and follow-up scheduling buffer to config; follow-ups must now be scheduled X days after the appointment requiring the follow-up
</commit_message>
<xml_diff>
--- a/SchedSimConfig.xlsx
+++ b/SchedSimConfig.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Patients</t>
   </si>
@@ -57,6 +57,12 @@
   </si>
   <si>
     <t>DaysInCycle</t>
+  </si>
+  <si>
+    <t>FollowUpBuffer</t>
+  </si>
+  <si>
+    <t>FollowUpProb</t>
   </si>
 </sst>
 </file>
@@ -419,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,10 +436,12 @@
     <col min="1" max="1" width="19" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="10" max="10" width="14" customWidth="1"/>
+    <col min="10" max="10" width="16.5703125" customWidth="1"/>
+    <col min="11" max="11" width="17.85546875" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -464,8 +472,14 @@
       <c r="J1" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="K1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>100</v>
       </c>
@@ -495,6 +509,12 @@
       </c>
       <c r="J2">
         <v>2</v>
+      </c>
+      <c r="K2">
+        <v>7</v>
+      </c>
+      <c r="L2">
+        <v>0.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes made to configurations and releasing slots based on day in the cycle
</commit_message>
<xml_diff>
--- a/SchedSimConfig.xlsx
+++ b/SchedSimConfig.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Patients</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>FollowUpProb</t>
+  </si>
+  <si>
+    <t>SlotsPerDay</t>
   </si>
 </sst>
 </file>
@@ -425,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,7 +444,7 @@
     <col min="12" max="12" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -478,8 +481,11 @@
       <c r="L1" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="M1" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>100</v>
       </c>
@@ -515,6 +521,9 @@
       </c>
       <c r="L2">
         <v>0.25</v>
+      </c>
+      <c r="M2">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>